<commit_message>
updated to add the 2 new params
</commit_message>
<xml_diff>
--- a/data/population_ghi_unemploment_yearwise_import export_africa_sheet.xlsx
+++ b/data/population_ghi_unemploment_yearwise_import export_africa_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haydencordeiro\Desktop\ADT project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C9B797-2974-4763-8E6E-CAB39250C834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA30F17-D898-4A66-9276-9451D1FCB41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,7 +201,7 @@
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -225,8 +225,11 @@
     <xf numFmtId="11" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -550,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2794,6 +2797,15 @@
       <c r="F64">
         <v>7.8146323529411763</v>
       </c>
+      <c r="G64" s="2">
+        <v>79.42</v>
+      </c>
+      <c r="H64" s="10">
+        <v>230</v>
+      </c>
+      <c r="I64" s="10">
+        <v>470</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated data for oil and employement
</commit_message>
<xml_diff>
--- a/data/population_ghi_unemploment_yearwise_import export_africa_sheet.xlsx
+++ b/data/population_ghi_unemploment_yearwise_import export_africa_sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haydencordeiro\Desktop\ADT project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA30F17-D898-4A66-9276-9451D1FCB41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9E1BFA-2809-46A8-81DF-6D981D533456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Year</t>
   </si>
@@ -55,6 +55,15 @@
   <si>
     <t>Export (US$ Thousand)</t>
   </si>
+  <si>
+    <t>NET OFFICIAL DEVELOPMENT ASSISTANCE AND AID</t>
+  </si>
+  <si>
+    <t>CREDIT RECEIVED FROM OTHER COUNTRIES IN BILLIONS</t>
+  </si>
+  <si>
+    <t>GASOLINE(USD)</t>
+  </si>
 </sst>
 </file>
 
@@ -66,7 +75,7 @@
     <numFmt numFmtId="166" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +117,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -201,7 +217,7 @@
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -228,7 +244,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -551,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N33" sqref="N2:N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,9 +589,11 @@
     <col min="9" max="9" width="18.44140625" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
     <col min="11" max="11" width="22.44140625" customWidth="1"/>
+    <col min="12" max="12" width="27.44140625" customWidth="1"/>
+    <col min="13" max="13" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,9 +627,17 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6"/>
-    </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1960</v>
       </c>
@@ -642,8 +671,17 @@
       <c r="K2" s="8">
         <v>-55000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L2">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="M2" s="6">
+        <v>-121248.90150000001</v>
+      </c>
+      <c r="N2" s="6">
+        <v>-0.38255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1961</v>
       </c>
@@ -677,8 +715,17 @@
       <c r="K3" s="8">
         <v>-55400000</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="M3" s="6">
+        <v>-120141.93769999999</v>
+      </c>
+      <c r="N3" s="6">
+        <v>-0.32140099999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1962</v>
       </c>
@@ -712,8 +759,17 @@
       <c r="K4" s="8">
         <v>-47200000</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="M4" s="6">
+        <v>-119858.62239999999</v>
+      </c>
+      <c r="N4" s="6">
+        <v>-0.32528099999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1963</v>
       </c>
@@ -747,8 +803,17 @@
       <c r="K5" s="8">
         <v>-47200000</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="M5" s="6">
+        <v>-121848.9387</v>
+      </c>
+      <c r="N5" s="6">
+        <v>-0.29672100000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1964</v>
       </c>
@@ -782,8 +847,17 @@
       <c r="K6" s="8">
         <v>-48300000</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>1.01</v>
+      </c>
+      <c r="M6" s="6">
+        <v>-108524.46339999999</v>
+      </c>
+      <c r="N6" s="6">
+        <v>-0.269731</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1965</v>
       </c>
@@ -817,8 +891,17 @@
       <c r="K7" s="8">
         <v>-48700000</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L7">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="M7" s="6">
+        <v>-107417.49950000001</v>
+      </c>
+      <c r="N7" s="6">
+        <v>-0.20858199999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1966</v>
       </c>
@@ -852,8 +935,17 @@
       <c r="K8" s="8">
         <v>-40500000</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>1.17</v>
+      </c>
+      <c r="M8" s="6">
+        <v>-107134.18429999999</v>
+      </c>
+      <c r="N8" s="6">
+        <v>-0.21246200000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1967</v>
       </c>
@@ -887,8 +979,17 @@
       <c r="K9" s="8">
         <v>-40500000</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L9">
+        <v>1.28</v>
+      </c>
+      <c r="M9" s="6">
+        <v>-109124.50049999999</v>
+      </c>
+      <c r="N9" s="6">
+        <v>-0.18390200000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1968</v>
       </c>
@@ -922,8 +1023,17 @@
       <c r="K10" s="8">
         <v>-41500000</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="M10" s="6">
+        <v>-95800.025219999996</v>
+      </c>
+      <c r="N10" s="6">
+        <v>-0.156912</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1969</v>
       </c>
@@ -957,8 +1067,17 @@
       <c r="K11" s="8">
         <v>-41900000</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L11">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="M11" s="6">
+        <v>-94693.061400000006</v>
+      </c>
+      <c r="N11" s="6">
+        <v>-9.5764000000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1970</v>
       </c>
@@ -992,8 +1111,17 @@
       <c r="K12" s="8">
         <v>-33700000</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>1.17</v>
+      </c>
+      <c r="M12" s="6">
+        <v>-94409.746109999993</v>
+      </c>
+      <c r="N12" s="6">
+        <v>-9.9643999999999996E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1971</v>
       </c>
@@ -1027,8 +1155,17 @@
       <c r="K13" s="8">
         <v>-33700000</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L13">
+        <v>1.36</v>
+      </c>
+      <c r="M13" s="6">
+        <v>-96400.062380000003</v>
+      </c>
+      <c r="N13" s="6">
+        <v>-7.1083999999999994E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1972</v>
       </c>
@@ -1062,8 +1199,17 @@
       <c r="K14" s="8">
         <v>-34800000</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>1.45</v>
+      </c>
+      <c r="M14" s="6">
+        <v>-83075.587069999994</v>
+      </c>
+      <c r="N14" s="6">
+        <v>-4.4094000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1973</v>
       </c>
@@ -1097,8 +1243,17 @@
       <c r="K15" s="8">
         <v>-35200000</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>1.8</v>
+      </c>
+      <c r="M15" s="6">
+        <v>-81968.623240000001</v>
+      </c>
+      <c r="N15" s="6">
+        <v>1.7055000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1974</v>
       </c>
@@ -1132,8 +1287,17 @@
       <c r="K16" s="8">
         <v>-26900000</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L16">
+        <v>2.6</v>
+      </c>
+      <c r="M16" s="6">
+        <v>-81685.307950000002</v>
+      </c>
+      <c r="N16" s="6">
+        <v>1.3174999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1975</v>
       </c>
@@ -1167,8 +1331,17 @@
       <c r="K17" s="8">
         <v>-27000000</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L17">
+        <v>3.5</v>
+      </c>
+      <c r="M17" s="6">
+        <v>-83675.624230000001</v>
+      </c>
+      <c r="N17" s="6">
+        <v>4.1735000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1976</v>
       </c>
@@ -1202,8 +1375,17 @@
       <c r="K18" s="8">
         <v>-28000000</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L18">
+        <v>3.23</v>
+      </c>
+      <c r="M18" s="6">
+        <v>-70351.148920000007</v>
+      </c>
+      <c r="N18" s="6">
+        <v>6.8724999999999994E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1977</v>
       </c>
@@ -1237,8 +1419,17 @@
       <c r="K19" s="8">
         <v>-28400000</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L19">
+        <v>3.85</v>
+      </c>
+      <c r="M19" s="6">
+        <v>-69244.185089999999</v>
+      </c>
+      <c r="N19" s="6">
+        <v>0.12987399999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1978</v>
       </c>
@@ -1272,8 +1463,17 @@
       <c r="K20" s="8">
         <v>-20200000</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L20">
+        <v>5.21</v>
+      </c>
+      <c r="M20" s="6">
+        <v>-68960.8698</v>
+      </c>
+      <c r="N20" s="6">
+        <v>0.12599399999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1979</v>
       </c>
@@ -1307,8 +1507,17 @@
       <c r="K21" s="8">
         <v>-20200000</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L21">
+        <v>6.66</v>
+      </c>
+      <c r="M21" s="6">
+        <v>-70951.186069999996</v>
+      </c>
+      <c r="N21" s="6">
+        <v>0.154554</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1980</v>
       </c>
@@ -1342,8 +1551,17 @@
       <c r="K22" s="8">
         <v>-21300000</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L22">
+        <v>7.72</v>
+      </c>
+      <c r="M22" s="6">
+        <v>-57626.710760000002</v>
+      </c>
+      <c r="N22" s="6">
+        <v>0.18154400000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1981</v>
       </c>
@@ -1377,8 +1595,17 @@
       <c r="K23" s="8">
         <v>-21600000</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L23">
+        <v>7.49</v>
+      </c>
+      <c r="M23" s="6">
+        <v>-56519.746930000001</v>
+      </c>
+      <c r="N23" s="6">
+        <v>0.24269299999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1982</v>
       </c>
@@ -1412,8 +1639,17 @@
       <c r="K24" s="8">
         <v>-13400000</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L24">
+        <v>7.86</v>
+      </c>
+      <c r="M24" s="6">
+        <v>-56236.431640000003</v>
+      </c>
+      <c r="N24" s="6">
+        <v>0.238813</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1983</v>
       </c>
@@ -1447,8 +1683,17 @@
       <c r="K25" s="8">
         <v>-13500000</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L25">
+        <v>7.58</v>
+      </c>
+      <c r="M25" s="6">
+        <v>-58226.747920000002</v>
+      </c>
+      <c r="N25" s="6">
+        <v>0.26737300000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1984</v>
       </c>
@@ -1482,8 +1727,17 @@
       <c r="K26" s="8">
         <v>-14500000</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L26">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="M26" s="6">
+        <v>-44902.27261</v>
+      </c>
+      <c r="N26" s="6">
+        <v>0.29436299999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1985</v>
       </c>
@@ -1517,8 +1771,17 @@
       <c r="K27" s="8">
         <v>-14900000</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L27">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="M27" s="6">
+        <v>-43795.308779999999</v>
+      </c>
+      <c r="N27" s="6">
+        <v>0.35551100000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1986</v>
       </c>
@@ -1552,8 +1815,17 @@
       <c r="K28" s="8">
         <v>-6680000</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L28">
+        <v>11.02</v>
+      </c>
+      <c r="M28" s="6">
+        <v>-43511.993490000001</v>
+      </c>
+      <c r="N28" s="6">
+        <v>0.35163100000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1987</v>
       </c>
@@ -1587,8 +1859,17 @@
       <c r="K29" s="8">
         <v>-6710000</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L29">
+        <v>12.81</v>
+      </c>
+      <c r="M29" s="6">
+        <v>-45502.30977</v>
+      </c>
+      <c r="N29" s="6">
+        <v>0.380191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1988</v>
       </c>
@@ -1622,8 +1903,17 @@
       <c r="K30" s="8">
         <v>-7750000</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L30">
+        <v>14.5</v>
+      </c>
+      <c r="M30" s="6">
+        <v>-32177.834449999998</v>
+      </c>
+      <c r="N30" s="6">
+        <v>0.40718100000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1989</v>
       </c>
@@ -1657,8 +1947,17 @@
       <c r="K31" s="8">
         <v>-8130000</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L31">
+        <v>15.5</v>
+      </c>
+      <c r="M31" s="6">
+        <v>-31070.870630000001</v>
+      </c>
+      <c r="N31" s="6">
+        <v>0.46833000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1990</v>
       </c>
@@ -1692,8 +1991,17 @@
       <c r="K32">
         <v>78828.661999999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L32">
+        <v>17.84</v>
+      </c>
+      <c r="M32" s="6">
+        <v>-30787.555339999999</v>
+      </c>
+      <c r="N32" s="6">
+        <v>0.46444999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1991</v>
       </c>
@@ -1727,8 +2035,17 @@
       <c r="K33">
         <v>71863.081999999995</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L33">
+        <v>17.82</v>
+      </c>
+      <c r="M33" s="6">
+        <v>-32777.871610000002</v>
+      </c>
+      <c r="N33" s="6">
+        <v>0.49301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1992</v>
       </c>
@@ -1762,8 +2079,17 @@
       <c r="K34">
         <v>2231145.406</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L34">
+        <v>19.239999999999998</v>
+      </c>
+      <c r="M34" s="6">
+        <v>-19453.3963</v>
+      </c>
+      <c r="N34">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1993</v>
       </c>
@@ -1797,8 +2123,17 @@
       <c r="K35">
         <v>2372597.7640000004</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L35">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="M35" s="6">
+        <v>-18346.43247</v>
+      </c>
+      <c r="N35">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1994</v>
       </c>
@@ -1832,8 +2167,17 @@
       <c r="K36">
         <v>2620872.4780000006</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L36">
+        <v>19.190000000000001</v>
+      </c>
+      <c r="M36" s="6">
+        <v>-18063.117180000001</v>
+      </c>
+      <c r="N36">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1995</v>
       </c>
@@ -1867,8 +2211,17 @@
       <c r="K37">
         <v>6255322.2939999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L37">
+        <v>18.64</v>
+      </c>
+      <c r="M37" s="6">
+        <v>-20053.43346</v>
+      </c>
+      <c r="N37">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1996</v>
       </c>
@@ -1902,8 +2255,17 @@
       <c r="K38">
         <v>7886224.3350000009</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L38">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="M38" s="6">
+        <v>-6728.9581449999996</v>
+      </c>
+      <c r="N38">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1997</v>
       </c>
@@ -1937,8 +2299,17 @@
       <c r="K39">
         <v>8296766.8059999961</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L39">
+        <v>14.9</v>
+      </c>
+      <c r="M39" s="6">
+        <v>-5621.9943169999997</v>
+      </c>
+      <c r="N39">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1998</v>
       </c>
@@ -1972,8 +2343,17 @@
       <c r="K40">
         <v>8009543.7199999988</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L40">
+        <v>14.48</v>
+      </c>
+      <c r="M40" s="6">
+        <v>-5338.6790270000001</v>
+      </c>
+      <c r="N40">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1999</v>
       </c>
@@ -2007,8 +2387,17 @@
       <c r="K41">
         <v>9096993.0329999998</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L41">
+        <v>13.23</v>
+      </c>
+      <c r="M41" s="6">
+        <v>-7328.9953029999997</v>
+      </c>
+      <c r="N41">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2000</v>
       </c>
@@ -2042,8 +2431,17 @@
       <c r="K42">
         <v>12495421.393247925</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L42">
+        <v>13.06</v>
+      </c>
+      <c r="M42">
+        <v>9135</v>
+      </c>
+      <c r="N42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2001</v>
       </c>
@@ -2077,8 +2475,17 @@
       <c r="K43">
         <v>11646401.438692028</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L43">
+        <v>14.29</v>
+      </c>
+      <c r="M43">
+        <v>8311</v>
+      </c>
+      <c r="N43">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2002</v>
       </c>
@@ -2112,8 +2519,17 @@
       <c r="K44">
         <v>13453823.025526304</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L44">
+        <v>19.05</v>
+      </c>
+      <c r="M44">
+        <v>7816</v>
+      </c>
+      <c r="N44">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2003</v>
       </c>
@@ -2147,8 +2563,17 @@
       <c r="K45">
         <v>15598582.279026113</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L45">
+        <v>24.88</v>
+      </c>
+      <c r="M45">
+        <v>9271</v>
+      </c>
+      <c r="N45">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2004</v>
       </c>
@@ -2182,8 +2607,17 @@
       <c r="K46">
         <v>17639388.170424521</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L46">
+        <v>26.49</v>
+      </c>
+      <c r="M46">
+        <v>9402</v>
+      </c>
+      <c r="N46">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2005</v>
       </c>
@@ -2217,8 +2651,17 @@
       <c r="K47">
         <v>19788814.732410166</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L47">
+        <v>32.840000000000003</v>
+      </c>
+      <c r="M47">
+        <v>12897</v>
+      </c>
+      <c r="N47">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2006</v>
       </c>
@@ -2252,8 +2695,17 @@
       <c r="K48">
         <v>31065184.161487054</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L48">
+        <v>41.2</v>
+      </c>
+      <c r="M48">
+        <v>14606</v>
+      </c>
+      <c r="N48">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2007</v>
       </c>
@@ -2287,8 +2739,17 @@
       <c r="K49">
         <v>34219894.205174908</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L49">
+        <v>36.17</v>
+      </c>
+      <c r="M49">
+        <v>20847</v>
+      </c>
+      <c r="N49">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2008</v>
       </c>
@@ -2322,8 +2783,17 @@
       <c r="K50">
         <v>43259630.429762773</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L50">
+        <v>40.26</v>
+      </c>
+      <c r="M50">
+        <v>20804</v>
+      </c>
+      <c r="N50">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2009</v>
       </c>
@@ -2357,8 +2827,17 @@
       <c r="K51">
         <v>41838937.966778494</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L51">
+        <v>44.31</v>
+      </c>
+      <c r="M51">
+        <v>31571</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2010</v>
       </c>
@@ -2392,8 +2871,17 @@
       <c r="K52">
         <v>60077956.472437307</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L52">
+        <v>44.36</v>
+      </c>
+      <c r="M52">
+        <v>37116</v>
+      </c>
+      <c r="N52">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2011</v>
       </c>
@@ -2427,8 +2915,17 @@
       <c r="K53">
         <v>72325759.653863475</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L53">
+        <v>47.33</v>
+      </c>
+      <c r="M53">
+        <v>27244</v>
+      </c>
+      <c r="N53">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2012</v>
       </c>
@@ -2462,8 +2959,17 @@
       <c r="K54">
         <v>75944887.738112509</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L54">
+        <v>46.76</v>
+      </c>
+      <c r="M54">
+        <v>47829</v>
+      </c>
+      <c r="N54">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2013</v>
       </c>
@@ -2497,8 +3003,17 @@
       <c r="K55">
         <v>76997064.96056363</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L55">
+        <v>47.7</v>
+      </c>
+      <c r="M55">
+        <v>48394</v>
+      </c>
+      <c r="N55">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2014</v>
       </c>
@@ -2532,8 +3047,17 @@
       <c r="K56">
         <v>74555107.939772487</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L56">
+        <v>46.46</v>
+      </c>
+      <c r="M56">
+        <v>56048</v>
+      </c>
+      <c r="N56">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2015</v>
       </c>
@@ -2567,8 +3091,17 @@
       <c r="K57">
         <v>68948168.174543768</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L57">
+        <v>44.77</v>
+      </c>
+      <c r="M57">
+        <v>46804</v>
+      </c>
+      <c r="N57">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2016</v>
       </c>
@@ -2602,8 +3135,17 @@
       <c r="K58">
         <v>62132954.958344154</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L58">
+        <v>44.32</v>
+      </c>
+      <c r="M58">
+        <v>82274</v>
+      </c>
+      <c r="N58">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2017</v>
       </c>
@@ -2637,8 +3179,17 @@
       <c r="K59">
         <v>67001541.885046229</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L59">
+        <v>49.57</v>
+      </c>
+      <c r="M59">
+        <v>74787</v>
+      </c>
+      <c r="N59">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2018</v>
       </c>
@@ -2672,8 +3223,17 @@
       <c r="K60">
         <v>77669133.054708242</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L60">
+        <v>50.89</v>
+      </c>
+      <c r="M60">
+        <v>65868</v>
+      </c>
+      <c r="N60">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2019</v>
       </c>
@@ -2707,8 +3267,17 @@
       <c r="K61">
         <v>71188007.499161556</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L61">
+        <v>53.08</v>
+      </c>
+      <c r="M61">
+        <v>76312</v>
+      </c>
+      <c r="N61">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2020</v>
       </c>
@@ -2742,8 +3311,17 @@
       <c r="K62">
         <v>55089138.426479578</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L62">
+        <v>66.89</v>
+      </c>
+      <c r="M62">
+        <v>83004</v>
+      </c>
+      <c r="N62">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2021</v>
       </c>
@@ -2777,8 +3355,17 @@
       <c r="K63">
         <v>64129944.018290378</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L63">
+        <v>62.29</v>
+      </c>
+      <c r="M63" s="6">
+        <v>73684.9064740459</v>
+      </c>
+      <c r="N63">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -2800,11 +3387,26 @@
       <c r="G64" s="2">
         <v>79.42</v>
       </c>
-      <c r="H64" s="10">
+      <c r="H64" s="2">
         <v>230</v>
       </c>
-      <c r="I64" s="10">
+      <c r="I64" s="2">
         <v>470</v>
+      </c>
+      <c r="J64" s="8">
+        <v>58033618.412437603</v>
+      </c>
+      <c r="K64" s="8">
+        <v>71067999.239628494</v>
+      </c>
+      <c r="L64" s="11">
+        <v>63</v>
+      </c>
+      <c r="M64" s="6">
+        <v>76987.404850845895</v>
+      </c>
+      <c r="N64">
+        <v>1.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>